<commit_message>
minor highlights in eichel data
</commit_message>
<xml_diff>
--- a/Eichel etal data/elife-52654-fig2-data4-v2.xlsx
+++ b/Eichel etal data/elife-52654-fig2-data4-v2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasia/Documents/Projects/PyCharm/Channel_coexpression/Eichel etal data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D45C7A0A-F083-A746-BDA1-E86E18E28EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6198C458-5003-D141-ADBC-4B01E7C2AE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{68497EE8-30C9-5B42-ADE7-60E936828CDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 2e" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -165,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,11 +468,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C929B1-06CA-A941-87DF-F92F638AEC1F}">
   <dimension ref="B1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">

</xml_diff>